<commit_message>
Graba Lat Long en Entregados
</commit_message>
<xml_diff>
--- a/FleetDelivery Modificaciones solicitadas.xlsx
+++ b/FleetDelivery Modificaciones solicitadas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Flutter\fleetdeliveryapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Flutter\fleetdeliveryapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4583A9B3-9AF3-4D97-9E65-C89D149812CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BB3FFA-E9DC-44DE-AF95-FD7AE296B876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2D167E44-E563-4DF9-9CAD-3636B941BCB8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Fecha</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>V.4 27/1/2022</t>
+  </si>
+  <si>
+    <t>Que cuando graba el envío, si es Entregado, grabe las coordenadas en nuevos campos Latitud2 y Longitud2</t>
+  </si>
+  <si>
+    <t>Que salga OrderId al lado de N° de Remito</t>
   </si>
 </sst>
 </file>
@@ -196,10 +202,10 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,7 +526,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3:E5"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.3"/>
@@ -587,7 +593,7 @@
         <v>44588</v>
       </c>
       <c r="D4" s="3"/>
-      <c r="E4" s="10"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
@@ -600,7 +606,7 @@
         <v>44588</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="9"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
@@ -624,16 +630,28 @@
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="3">
+        <v>44656</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3">
+        <v>44658</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
+    <row r="10" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>44656</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3">
+        <v>44658</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>

</xml_diff>